<commit_message>
info for flowchart, and organizing dataprocessing script
</commit_message>
<xml_diff>
--- a/data/country_info.xlsx
+++ b/data/country_info.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cscaff/Documents/GitHub/weirdChildes/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{66BC9810-DAB0-F24C-AAC6-4E3B9A16F8EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D72549E2-FC7C-9E48-B2D3-CB16C96D23E1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16120" xr2:uid="{544F1760-8C40-8D4C-9C77-745FFDE93F04}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15820" xr2:uid="{544F1760-8C40-8D4C-9C77-745FFDE93F04}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="69">
   <si>
     <t>Argentina</t>
   </si>
@@ -169,9 +168,6 @@
     <t>United_States</t>
   </si>
   <si>
-    <t>country</t>
-  </si>
-  <si>
     <t>n_corpora</t>
   </si>
   <si>
@@ -225,6 +221,18 @@
   <si>
     <t>yes</t>
   </si>
+  <si>
+    <t>country annotation</t>
+  </si>
+  <si>
+    <t>country childes</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>middle_class</t>
+  </si>
 </sst>
 </file>
 
@@ -246,18 +254,18 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="16"/>
-      <color rgb="FF0B1E2D"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Lucida Grande"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -279,13 +287,13 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -308,7 +316,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -351,7 +359,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -394,7 +402,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -437,7 +445,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -480,7 +488,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -523,7 +531,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -566,7 +574,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -609,7 +617,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -652,7 +660,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -695,7 +703,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -738,7 +746,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -781,7 +789,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -824,7 +832,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -867,7 +875,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -910,7 +918,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -953,7 +961,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -996,7 +1004,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1039,7 +1047,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1082,7 +1090,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1125,7 +1133,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1168,7 +1176,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1211,7 +1219,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1254,7 +1262,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1297,7 +1305,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1340,7 +1348,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1383,7 +1391,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1426,7 +1434,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1469,7 +1477,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1512,7 +1520,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1555,7 +1563,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1598,7 +1606,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1641,7 +1649,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1684,7 +1692,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1727,7 +1735,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1770,7 +1778,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1813,7 +1821,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1856,7 +1864,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1899,7 +1907,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1942,7 +1950,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -1985,7 +1993,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2028,7 +2036,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2071,7 +2079,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2114,7 +2122,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2157,7 +2165,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2200,7 +2208,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2243,7 +2251,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2286,7 +2294,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2329,7 +2337,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2372,7 +2380,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2415,7 +2423,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2458,7 +2466,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2501,7 +2509,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2544,7 +2552,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2587,7 +2595,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2630,7 +2638,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2673,7 +2681,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2716,7 +2724,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2759,7 +2767,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2802,7 +2810,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2845,7 +2853,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2888,7 +2896,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2931,7 +2939,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2974,7 +2982,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3017,7 +3025,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3060,7 +3068,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3103,7 +3111,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3146,7 +3154,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3189,7 +3197,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3232,7 +3240,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3275,7 +3283,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3318,7 +3326,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3361,7 +3369,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3404,7 +3412,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3447,7 +3455,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3490,7 +3498,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3533,7 +3541,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3576,7 +3584,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3619,7 +3627,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3662,7 +3670,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3705,7 +3713,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3748,7 +3756,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3791,7 +3799,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3834,7 +3842,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3877,7 +3885,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3920,7 +3928,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>34</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3963,7 +3971,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4006,7 +4014,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4049,7 +4057,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4092,7 +4100,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4135,7 +4143,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>43</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4178,7 +4186,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4221,7 +4229,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4264,7 +4272,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4307,7 +4315,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4350,7 +4358,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4393,7 +4401,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4436,7 +4444,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4479,7 +4487,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4522,7 +4530,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4565,7 +4573,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4608,7 +4616,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4651,7 +4659,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4694,7 +4702,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4737,7 +4745,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4780,7 +4788,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4823,7 +4831,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4866,7 +4874,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4909,7 +4917,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4952,7 +4960,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -4995,7 +5003,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5038,7 +5046,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5081,7 +5089,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5124,7 +5132,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5167,7 +5175,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5210,7 +5218,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5253,7 +5261,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5296,7 +5304,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5339,7 +5347,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5382,7 +5390,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5425,7 +5433,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5468,7 +5476,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5511,7 +5519,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5554,7 +5562,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5597,7 +5605,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5640,7 +5648,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5683,7 +5691,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5726,7 +5734,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5769,7 +5777,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5812,7 +5820,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5855,7 +5863,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5898,7 +5906,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5941,7 +5949,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -5984,7 +5992,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6027,7 +6035,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6070,7 +6078,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6113,7 +6121,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6156,7 +6164,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6199,7 +6207,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6242,7 +6250,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6285,7 +6293,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6328,7 +6336,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6371,7 +6379,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6414,7 +6422,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6457,7 +6465,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6500,7 +6508,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6543,7 +6551,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6586,7 +6594,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6629,7 +6637,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6672,7 +6680,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6715,7 +6723,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6758,7 +6766,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6801,7 +6809,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6844,7 +6852,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6887,7 +6895,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>39</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6930,7 +6938,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -6973,7 +6981,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -7016,7 +7024,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>40</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -7059,7 +7067,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -7102,7 +7110,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -7145,7 +7153,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -7188,7 +7196,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -7231,7 +7239,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>42</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -7274,7 +7282,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -7317,7 +7325,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -7360,7 +7368,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -7403,7 +7411,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -7446,7 +7454,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -7489,7 +7497,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -7532,7 +7540,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -7575,7 +7583,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -7618,7 +7626,7 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>47</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -7659,30 +7667,25 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2201" name="AutoShape 153" descr="Australia flag">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BC7B129-F08C-C942-8D3B-BEAE67C8C754}"/>
+        <xdr:cNvPr id="250" name="AutoShape 153" descr="Australia flag">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{539C8844-B353-CD4C-91B9-96834954241C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -8012,731 +8015,850 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3220AFF8-AA48-7440-948B-D2C3B57EACC2}">
-  <dimension ref="A1:Q97"/>
+  <dimension ref="A1:R97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="9.1640625" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="26.33203125" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" t="s">
+        <v>57</v>
+      </c>
+      <c r="P1" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>59</v>
+      </c>
+      <c r="R1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>63</v>
       </c>
-      <c r="D1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" t="s">
-        <v>49</v>
-      </c>
-      <c r="F1" t="s">
-        <v>50</v>
-      </c>
-      <c r="G1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J1" t="s">
-        <v>54</v>
-      </c>
-      <c r="K1" t="s">
-        <v>55</v>
-      </c>
-      <c r="L1" t="s">
-        <v>56</v>
-      </c>
-      <c r="M1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N1" t="s">
-        <v>58</v>
-      </c>
-      <c r="O1" t="s">
-        <v>59</v>
-      </c>
-      <c r="P1" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>61</v>
+      <c r="E2" s="3">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" t="s">
+        <v>64</v>
+      </c>
+      <c r="N2" t="s">
+        <v>67</v>
+      </c>
+      <c r="O2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>67</v>
+      </c>
+      <c r="R2" t="s">
+        <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="3" spans="1:18" ht="20" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
         <v>64</v>
       </c>
+      <c r="D3" s="1">
+        <v>1961</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:18" ht="20" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1961</v>
+      </c>
+      <c r="E4" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="20" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" s="1">
+    </row>
+    <row r="6" spans="1:18" ht="20" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" s="1">
         <v>1961</v>
       </c>
+      <c r="E6" s="3">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="7" spans="1:18" ht="20" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="20" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="3">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C4" s="1">
+    </row>
+    <row r="9" spans="1:18" ht="20" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1995</v>
+      </c>
+      <c r="E9" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="20" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="1">
         <v>1961</v>
       </c>
+      <c r="E10" s="3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="5" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="11" spans="1:18" ht="20" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="20" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2010</v>
+      </c>
+      <c r="E12" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="20" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1961</v>
+      </c>
+      <c r="E13" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="20" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1961</v>
+      </c>
+      <c r="E14" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="20" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1961</v>
+      </c>
+      <c r="E15" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="20" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1996</v>
+      </c>
+      <c r="E16" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1961</v>
+      </c>
+      <c r="E17" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" s="1">
+        <v>1961</v>
+      </c>
+      <c r="E21" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="1">
+        <v>2010</v>
+      </c>
+      <c r="E22" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="1">
+        <v>1962</v>
+      </c>
+      <c r="E23" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1964</v>
+      </c>
+      <c r="E25" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" t="s">
+        <v>64</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1996</v>
+      </c>
+      <c r="E26" s="3">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="27" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>63</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
+        <v>27</v>
+      </c>
+      <c r="C29" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="D29" s="1">
+        <v>1994</v>
+      </c>
+      <c r="E29" s="3">
+        <v>3</v>
+      </c>
     </row>
-    <row r="6" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="30" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D30" s="1">
+        <v>1961</v>
+      </c>
+      <c r="E30" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" t="s">
+        <v>64</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1961</v>
+      </c>
+      <c r="E31" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="1"/>
+      <c r="E32" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>31</v>
+      </c>
+      <c r="C33" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="1">
+        <v>1996</v>
+      </c>
+      <c r="E33" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C34" t="s">
+        <v>64</v>
+      </c>
+      <c r="D34" s="1">
+        <v>1961</v>
+      </c>
+      <c r="E34" s="3">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="1">
+    </row>
+    <row r="35" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" t="s">
+        <v>63</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" t="s">
+        <v>63</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" t="s">
+        <v>63</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" t="s">
+        <v>64</v>
+      </c>
+      <c r="D39" s="1">
+        <v>2010</v>
+      </c>
+      <c r="E39" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="1">
         <v>1961</v>
       </c>
+      <c r="E41" s="3">
+        <v>28</v>
+      </c>
     </row>
-    <row r="7" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="42" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="1">
+        <v>1961</v>
+      </c>
+      <c r="E42" s="3">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="43" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>41</v>
+      </c>
+      <c r="C43" t="s">
         <v>64</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="D43" s="1">
+        <v>1961</v>
+      </c>
+      <c r="E43" s="3">
+        <v>1</v>
+      </c>
     </row>
-    <row r="8" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="44" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" t="s">
+        <v>63</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>43</v>
+      </c>
+      <c r="C45" t="s">
+        <v>63</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>44</v>
+      </c>
+      <c r="C46" t="s">
         <v>64</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="D46" s="1">
+        <v>1961</v>
+      </c>
+      <c r="E46" s="3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="9" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>65</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1995</v>
+    <row r="47" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
+        <v>45</v>
+      </c>
+      <c r="C47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D47" s="1">
+        <v>1961</v>
+      </c>
+      <c r="E47" s="3">
+        <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="1">
+    <row r="48" spans="2:5" ht="20" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48" s="1">
         <v>1961</v>
       </c>
+      <c r="E48" s="3">
+        <v>46</v>
+      </c>
     </row>
-    <row r="11" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="1"/>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="E49">
+        <f>SUM(E2:E48)</f>
+        <v>259</v>
+      </c>
     </row>
-    <row r="12" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2010</v>
-      </c>
+    <row r="60" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D60" s="2"/>
     </row>
-    <row r="13" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>65</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1961</v>
-      </c>
+    <row r="61" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D61" s="2"/>
     </row>
-    <row r="14" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1961</v>
-      </c>
+    <row r="62" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D62" s="2"/>
     </row>
-    <row r="15" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" t="s">
-        <v>65</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1961</v>
-      </c>
+    <row r="63" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D63" s="2"/>
     </row>
-    <row r="16" spans="1:17" ht="20" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" t="s">
-        <v>65</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1996</v>
-      </c>
+    <row r="64" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D64" s="2"/>
     </row>
-    <row r="17" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="1">
-        <v>1961</v>
-      </c>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D65" s="2"/>
     </row>
-    <row r="18" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" t="s">
-        <v>64</v>
-      </c>
-      <c r="C18" s="1"/>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D66" s="2"/>
     </row>
-    <row r="19" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="1"/>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D67" s="2"/>
     </row>
-    <row r="20" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" t="s">
-        <v>64</v>
-      </c>
-      <c r="C20" s="1"/>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D68" s="2"/>
     </row>
-    <row r="21" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B21" t="s">
-        <v>65</v>
-      </c>
-      <c r="C21" s="1">
-        <v>1961</v>
-      </c>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D69" s="2"/>
     </row>
-    <row r="22" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" s="1">
-        <v>2010</v>
-      </c>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D70" s="2"/>
     </row>
-    <row r="23" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>65</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1962</v>
-      </c>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D71" s="2"/>
     </row>
-    <row r="24" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>64</v>
-      </c>
-      <c r="C24" s="1"/>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D72" s="2"/>
     </row>
-    <row r="25" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" t="s">
-        <v>65</v>
-      </c>
-      <c r="C25" s="1">
-        <v>1964</v>
-      </c>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D73" s="2"/>
     </row>
-    <row r="26" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" s="1">
-        <v>1996</v>
-      </c>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D74" s="2"/>
     </row>
-    <row r="27" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>25</v>
-      </c>
-      <c r="B27" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="1"/>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D75" s="2"/>
     </row>
-    <row r="28" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>26</v>
-      </c>
-      <c r="B28" t="s">
-        <v>64</v>
-      </c>
-      <c r="C28" s="1"/>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D76" s="2"/>
     </row>
-    <row r="29" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" t="s">
-        <v>65</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1994</v>
-      </c>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D77" s="2"/>
     </row>
-    <row r="30" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>28</v>
-      </c>
-      <c r="B30" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" s="1">
-        <v>1961</v>
-      </c>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D78" s="2"/>
     </row>
-    <row r="31" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>29</v>
-      </c>
-      <c r="B31" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="1">
-        <v>1961</v>
-      </c>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D79" s="2"/>
     </row>
-    <row r="32" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="1"/>
+    <row r="80" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D80" s="2"/>
     </row>
-    <row r="33" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>31</v>
-      </c>
-      <c r="B33" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="1">
-        <v>1996</v>
-      </c>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D81" s="2"/>
     </row>
-    <row r="34" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>32</v>
-      </c>
-      <c r="B34" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" s="1">
-        <v>1961</v>
-      </c>
+    <row r="82" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D82" s="2"/>
     </row>
-    <row r="35" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C35" s="1"/>
+    <row r="83" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D83" s="2"/>
     </row>
-    <row r="36" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>34</v>
-      </c>
-      <c r="B36" t="s">
-        <v>64</v>
-      </c>
-      <c r="C36" s="1"/>
+    <row r="84" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D84" s="2"/>
     </row>
-    <row r="37" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C37" s="1"/>
+    <row r="85" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D85" s="2"/>
     </row>
-    <row r="38" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" t="s">
-        <v>64</v>
-      </c>
-      <c r="C38" s="1"/>
+    <row r="86" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D86" s="2"/>
     </row>
-    <row r="39" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>37</v>
-      </c>
-      <c r="B39" t="s">
-        <v>65</v>
-      </c>
-      <c r="C39" s="1">
-        <v>2010</v>
-      </c>
+    <row r="87" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D87" s="2"/>
     </row>
-    <row r="40" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" t="s">
-        <v>64</v>
-      </c>
-      <c r="C40" s="1"/>
+    <row r="88" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D88" s="2"/>
     </row>
-    <row r="41" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41" t="s">
-        <v>65</v>
-      </c>
-      <c r="C41" s="1">
-        <v>1961</v>
-      </c>
+    <row r="89" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D89" s="2"/>
     </row>
-    <row r="42" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>40</v>
-      </c>
-      <c r="B42" t="s">
-        <v>65</v>
-      </c>
-      <c r="C42" s="1">
-        <v>1961</v>
-      </c>
+    <row r="90" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D90" s="2"/>
     </row>
-    <row r="43" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>41</v>
-      </c>
-      <c r="B43" t="s">
-        <v>65</v>
-      </c>
-      <c r="C43" s="1">
-        <v>1961</v>
-      </c>
+    <row r="91" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D91" s="2"/>
     </row>
-    <row r="44" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>42</v>
-      </c>
-      <c r="B44" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" s="1"/>
+    <row r="92" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D92" s="2"/>
     </row>
-    <row r="45" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>43</v>
-      </c>
-      <c r="B45" t="s">
-        <v>64</v>
-      </c>
-      <c r="C45" s="1"/>
+    <row r="93" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D93" s="2"/>
     </row>
-    <row r="46" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>44</v>
-      </c>
-      <c r="B46" t="s">
-        <v>65</v>
-      </c>
-      <c r="C46" s="1">
-        <v>1961</v>
-      </c>
+    <row r="94" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D94" s="2"/>
     </row>
-    <row r="47" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>45</v>
-      </c>
-      <c r="B47" t="s">
-        <v>65</v>
-      </c>
-      <c r="C47" s="1">
-        <v>1961</v>
-      </c>
+    <row r="95" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D95" s="2"/>
     </row>
-    <row r="48" spans="1:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>46</v>
-      </c>
-      <c r="B48" t="s">
-        <v>65</v>
-      </c>
-      <c r="C48" s="1">
-        <v>1961</v>
-      </c>
+    <row r="96" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D96" s="2"/>
     </row>
-    <row r="60" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C60" s="3"/>
-    </row>
-    <row r="61" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C61" s="3"/>
-    </row>
-    <row r="62" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C62" s="3"/>
-    </row>
-    <row r="63" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C63" s="3"/>
-    </row>
-    <row r="64" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C64" s="3"/>
-    </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C65" s="3"/>
-    </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C66" s="3"/>
-    </row>
-    <row r="67" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C67" s="3"/>
-    </row>
-    <row r="68" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C68" s="3"/>
-    </row>
-    <row r="69" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C69" s="3"/>
-    </row>
-    <row r="70" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C70" s="3"/>
-    </row>
-    <row r="71" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C71" s="3"/>
-    </row>
-    <row r="72" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C72" s="3"/>
-    </row>
-    <row r="73" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C73" s="3"/>
-    </row>
-    <row r="74" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C74" s="3"/>
-    </row>
-    <row r="75" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C75" s="3"/>
-    </row>
-    <row r="76" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C76" s="3"/>
-    </row>
-    <row r="77" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C77" s="3"/>
-    </row>
-    <row r="78" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C78" s="3"/>
-    </row>
-    <row r="79" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C79" s="3"/>
-    </row>
-    <row r="80" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C80" s="3"/>
-    </row>
-    <row r="81" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C81" s="3"/>
-    </row>
-    <row r="82" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C82" s="3"/>
-    </row>
-    <row r="83" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C83" s="3"/>
-    </row>
-    <row r="84" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C84" s="3"/>
-    </row>
-    <row r="85" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C85" s="3"/>
-    </row>
-    <row r="86" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C86" s="3"/>
-    </row>
-    <row r="87" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C87" s="3"/>
-    </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C88" s="3"/>
-    </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C89" s="3"/>
-    </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C90" s="3"/>
-    </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C91" s="3"/>
-    </row>
-    <row r="92" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C92" s="3"/>
-    </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C93" s="3"/>
-    </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C94" s="3"/>
-    </row>
-    <row r="95" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C95" s="3"/>
-    </row>
-    <row r="96" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C96" s="3"/>
-    </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C97" s="3"/>
+    <row r="97" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D97" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C8617D9-5139-2048-A583-5A03A9CA87DC}">
-  <dimension ref="C2:D42"/>
-  <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B38" sqref="A1:B38"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="2" spans="3:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="D2" s="2"/>
-    </row>
-    <row r="3" spans="3:4" ht="20" x14ac:dyDescent="0.2">
-      <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
-    </row>
-    <row r="42" spans="3:3" ht="20" x14ac:dyDescent="0.2">
-      <c r="C42" s="1"/>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A38" r:id="rId1" display="https://www.oecd.org/unitedstates/" xr:uid="{FD8436B9-9BF7-744D-91BB-2486B5906938}"/>
-    <hyperlink ref="A37" r:id="rId2" display="https://www.oecd.org/unitedkingdom/" xr:uid="{A10D75CA-5F76-9B43-BF57-7BF85CDFC692}"/>
-    <hyperlink ref="A36" r:id="rId3" display="https://www.oecd.org/turkiye/" xr:uid="{55652918-1745-2E46-A20C-A0BB535DF443}"/>
-    <hyperlink ref="A35" r:id="rId4" display="https://www.oecd.org/switzerland/" xr:uid="{619CFE48-D794-894D-B266-AD6469C8A559}"/>
-    <hyperlink ref="A34" r:id="rId5" display="https://www.oecd.org/sweden/" xr:uid="{7B579AEE-CDA3-784E-B166-B842D278D655}"/>
-    <hyperlink ref="A33" r:id="rId6" display="https://www.oecd.org/spain/" xr:uid="{CFB3BD61-D1B4-AF43-945D-976D0BBFF41D}"/>
-    <hyperlink ref="A32" r:id="rId7" display="https://www.oecd.org/slovenia/" xr:uid="{00BAB718-878F-1040-B13C-92513E499EED}"/>
-    <hyperlink ref="A31" r:id="rId8" display="https://www.oecd.org/slovakia/" xr:uid="{C871159C-8906-D94E-8FE1-8BA804AA20AD}"/>
-    <hyperlink ref="A30" r:id="rId9" display="https://www.oecd.org/portugal/" xr:uid="{25A3D651-4105-8643-BC82-44B4EBCC0066}"/>
-    <hyperlink ref="A29" r:id="rId10" display="https://www.oecd.org/poland/" xr:uid="{9CFA2A50-67C6-A44F-8873-657D34C315A2}"/>
-    <hyperlink ref="A28" r:id="rId11" display="https://www.oecd.org/norway/" xr:uid="{D68D6503-CBCD-2749-8E21-0861F8E92FBB}"/>
-    <hyperlink ref="A27" r:id="rId12" display="https://www.oecd.org/newzealand/" xr:uid="{202365D2-3C7F-BB42-A3B9-FAF1E78AE9DC}"/>
-    <hyperlink ref="A26" r:id="rId13" display="https://www.oecd.org/netherlands/" xr:uid="{FA5736F6-BA83-C943-8BF8-1D5345C0CFCD}"/>
-    <hyperlink ref="A25" r:id="rId14" display="https://www.oecd.org/mexico/" xr:uid="{903DE123-C510-B44F-B08A-1220BF282C67}"/>
-    <hyperlink ref="A24" r:id="rId15" display="https://www.oecd.org/luxembourg/" xr:uid="{C79AAC5C-80DF-134E-82C7-22DF2B08DE01}"/>
-    <hyperlink ref="A23" r:id="rId16" display="https://www.oecd.org/lithuania/" xr:uid="{6756F02D-7C9F-574C-A93B-C82BFCF04A3C}"/>
-    <hyperlink ref="A22" r:id="rId17" display="https://www.oecd.org/latvia/" xr:uid="{EDC9B9BA-5489-6B48-A6B8-961BA3F4AFC4}"/>
-    <hyperlink ref="A21" r:id="rId18" display="https://www.oecd.org/korea/" xr:uid="{BB1F2ED7-19E2-A745-97CC-A92369097A93}"/>
-    <hyperlink ref="A20" r:id="rId19" display="https://www.oecd.org/japan/" xr:uid="{B7BE39B8-32C9-4248-87F8-E0D849212611}"/>
-    <hyperlink ref="A19" r:id="rId20" display="https://www.oecd.org/italy/" xr:uid="{F3CAE1FD-C007-E44B-B4E9-C2D6E2E9F50A}"/>
-    <hyperlink ref="A18" r:id="rId21" display="https://www.oecd.org/israel/" xr:uid="{973A139D-AAD8-6140-8AF2-EED64EADEC65}"/>
-    <hyperlink ref="A17" r:id="rId22" display="https://www.oecd.org/ireland/" xr:uid="{9A1A3E92-4597-8543-BDEA-A0773D30644B}"/>
-    <hyperlink ref="A16" r:id="rId23" display="https://www.oecd.org/iceland/" xr:uid="{329D30B6-EE7F-A247-8369-72E5AB2B1438}"/>
-    <hyperlink ref="A15" r:id="rId24" display="https://www.oecd.org/hungary/" xr:uid="{DE70901C-407A-F146-8552-D9C5AED659D7}"/>
-    <hyperlink ref="A14" r:id="rId25" display="https://www.oecd.org/greece/" xr:uid="{0CC38F31-775F-BD41-B176-D73E756B401B}"/>
-    <hyperlink ref="A13" r:id="rId26" display="https://www.oecd.org/germany/" xr:uid="{A998A4D8-48D9-EB4E-99BB-78C864284628}"/>
-    <hyperlink ref="A12" r:id="rId27" display="https://www.oecd.org/france" xr:uid="{10B0DEF2-2EF3-1D48-9184-C4E6000F82B6}"/>
-    <hyperlink ref="A11" r:id="rId28" display="https://www.oecd.org/finland/" xr:uid="{47AA340F-5D88-534A-BD1A-61E2C7E6F2B3}"/>
-    <hyperlink ref="A10" r:id="rId29" display="https://www.oecd.org/estonia/" xr:uid="{35E70DFB-2030-B740-B536-87D7935641CE}"/>
-    <hyperlink ref="A9" r:id="rId30" display="https://www.oecd.org/denmark/" xr:uid="{13932F39-371D-C142-AA88-10E6BFD9DD88}"/>
-    <hyperlink ref="A8" r:id="rId31" display="https://www.oecd.org/czech/" xr:uid="{2642F591-C4B7-D649-A60F-AAE69E5797F8}"/>
-    <hyperlink ref="A7" r:id="rId32" display="https://www.oecd.org/costarica/" xr:uid="{C2988370-22E0-5B4B-893A-73887FBE33A8}"/>
-    <hyperlink ref="A6" r:id="rId33" display="https://www.oecd.org/colombia/" xr:uid="{0D02912A-CD85-B24A-803E-D11BA5651150}"/>
-    <hyperlink ref="A5" r:id="rId34" display="https://www.oecd.org/chile" xr:uid="{013BA4C8-FAC3-334E-A330-E3DEF2504B4C}"/>
-    <hyperlink ref="A4" r:id="rId35" display="https://www.oecd.org/canada" xr:uid="{CED7AAA3-1663-5944-A540-AE4E5F5ED280}"/>
-    <hyperlink ref="A3" r:id="rId36" display="https://www.oecd.org/belgium" xr:uid="{65DE5A46-92C5-7841-8D03-78A6F60EA66C}"/>
-    <hyperlink ref="A2" r:id="rId37" display="https://www.oecd.org/austria" xr:uid="{ACBD8636-E84A-A64E-BC89-7D8C1BFA0588}"/>
-    <hyperlink ref="A1" r:id="rId38" display="https://www.oecd.org/australia" xr:uid="{1A0E5034-85B9-D446-B663-D72F107C584D}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId39"/>
-</worksheet>
 </file>
</xml_diff>